<commit_message>
Fix paths after repo rename and update for resubmission
all paths have been updated to cessationStability, and model content has been updated to go with the paper resubmission.
</commit_message>
<xml_diff>
--- a/data/India2010/modeledPrevalenceInHealthyContactsOfWPV1Cases.xlsx
+++ b/data/India2010/modeledPrevalenceInHealthyContactsOfWPV1Cases.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfamulare\Dropbox (IDM)\VaccineNetworkTransmissionPaper\data\India2010\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfamulare\Dropbox (IDM)\VaccineNetworkTransmissionPaper\revisedSupplement\data\India2010\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="7740"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="7740" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="immunity" sheetId="1" r:id="rId1"/>
+    <sheet name="WPV1" sheetId="2" r:id="rId2"/>
+    <sheet name="WPV3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>doses</t>
   </si>
@@ -57,6 +59,27 @@
   </si>
   <si>
     <t>11 day estimated WPV shedding duration of healthy contacts from Grassly2010</t>
+  </si>
+  <si>
+    <t>daysAfterParalysis</t>
+  </si>
+  <si>
+    <t>contactSampleSize</t>
+  </si>
+  <si>
+    <t>contactPercent</t>
+  </si>
+  <si>
+    <t>contactPositive</t>
+  </si>
+  <si>
+    <t>indexPercent</t>
+  </si>
+  <si>
+    <t>indexSampleSize</t>
+  </si>
+  <si>
+    <t>indexPositive</t>
   </si>
 </sst>
 </file>
@@ -410,13 +433,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -439,7 +462,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -462,7 +485,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -483,6 +506,732 @@
       </c>
       <c r="G3" t="s">
         <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1.7</v>
+      </c>
+      <c r="C2">
+        <v>1271</v>
+      </c>
+      <c r="D2">
+        <f>ROUND(B2/100*C2,0)</f>
+        <v>22</v>
+      </c>
+      <c r="E2">
+        <v>0.8</v>
+      </c>
+      <c r="F2">
+        <v>84681</v>
+      </c>
+      <c r="G2">
+        <f>ROUND(E2/100*F2,0)</f>
+        <v>677</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>0.8</v>
+      </c>
+      <c r="C3">
+        <v>2255</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D14" si="0">ROUND(B3/100*C3,0)</f>
+        <v>18</v>
+      </c>
+      <c r="E3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F3">
+        <v>51331</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G14" si="1">ROUND(E3/100*F3,0)</f>
+        <v>282</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>0.8</v>
+      </c>
+      <c r="C4">
+        <v>2261</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E4">
+        <v>0.5</v>
+      </c>
+      <c r="F4">
+        <v>7779</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>0.7</v>
+      </c>
+      <c r="C5">
+        <v>2080</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>0.37</v>
+      </c>
+      <c r="F5">
+        <v>4362</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>0.7</v>
+      </c>
+      <c r="C6">
+        <v>1549</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>0.4</v>
+      </c>
+      <c r="F6">
+        <v>3274</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>39</v>
+      </c>
+      <c r="B7">
+        <v>0.5</v>
+      </c>
+      <c r="C7">
+        <v>1106</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>0.38</v>
+      </c>
+      <c r="F7">
+        <v>1744</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>46</v>
+      </c>
+      <c r="B8">
+        <v>0.7</v>
+      </c>
+      <c r="C8">
+        <v>910</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>0.25</v>
+      </c>
+      <c r="F8">
+        <v>1300</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>53</v>
+      </c>
+      <c r="B9">
+        <v>0.7</v>
+      </c>
+      <c r="C9">
+        <v>599</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>0.13</v>
+      </c>
+      <c r="F9">
+        <v>886</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>60</v>
+      </c>
+      <c r="B10">
+        <v>0.25</v>
+      </c>
+      <c r="C10">
+        <v>406</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0.25</v>
+      </c>
+      <c r="F10">
+        <v>461</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>67</v>
+      </c>
+      <c r="B11">
+        <v>0.7</v>
+      </c>
+      <c r="C11">
+        <v>289</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>55</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>74</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>243</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>25</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>81</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>163</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>22</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>88</v>
+      </c>
+      <c r="B14">
+        <v>0.3</v>
+      </c>
+      <c r="C14">
+        <v>741</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1.9</v>
+      </c>
+      <c r="C2">
+        <v>1271</v>
+      </c>
+      <c r="D2">
+        <f>ROUND(B2/100*C2,0)</f>
+        <v>24</v>
+      </c>
+      <c r="E2">
+        <v>0.95</v>
+      </c>
+      <c r="F2">
+        <v>84681</v>
+      </c>
+      <c r="G2">
+        <f>ROUND(E2/100*F2,0)</f>
+        <v>804</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>0.3</v>
+      </c>
+      <c r="C3">
+        <v>2255</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D14" si="0">ROUND(B3/100*C3,0)</f>
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F3">
+        <v>51331</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G14" si="1">ROUND(E3/100*F3,0)</f>
+        <v>298</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>0.9</v>
+      </c>
+      <c r="C4">
+        <v>2261</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F4">
+        <v>7779</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2080</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="E5">
+        <v>0.5</v>
+      </c>
+      <c r="F5">
+        <v>4362</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1549</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>0.3</v>
+      </c>
+      <c r="F6">
+        <v>3274</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>39</v>
+      </c>
+      <c r="B7">
+        <v>0.4</v>
+      </c>
+      <c r="C7">
+        <v>1106</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>0.2</v>
+      </c>
+      <c r="F7">
+        <v>1744</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>46</v>
+      </c>
+      <c r="B8">
+        <v>0.5</v>
+      </c>
+      <c r="C8">
+        <v>910</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>0.2</v>
+      </c>
+      <c r="F8">
+        <v>1300</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>53</v>
+      </c>
+      <c r="B9">
+        <v>0.2</v>
+      </c>
+      <c r="C9">
+        <v>599</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0.35</v>
+      </c>
+      <c r="F9">
+        <v>886</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>60</v>
+      </c>
+      <c r="B10">
+        <v>0.25</v>
+      </c>
+      <c r="C10">
+        <v>406</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0.25</v>
+      </c>
+      <c r="F10">
+        <v>461</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>67</v>
+      </c>
+      <c r="B11">
+        <v>0.7</v>
+      </c>
+      <c r="C11">
+        <v>289</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>55</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>74</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>243</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>25</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>81</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>163</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>88</v>
+      </c>
+      <c r="B14">
+        <v>0.5</v>
+      </c>
+      <c r="C14">
+        <v>741</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>